<commit_message>
MOVPE STO workflow - refinements
</commit_message>
<xml_diff>
--- a/movpe_STO/datafile.xlsx
+++ b/movpe_STO/datafile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="263">
   <si>
     <t xml:space="preserve">########## start Header ##########</t>
   </si>
@@ -95,706 +95,706 @@
     <t xml:space="preserve">Activity Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2 Argon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22-01-21-MA-255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarragona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-08-25 10:33:25.013+02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epitaxy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movpe sto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">giorgio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STO:La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 x STO undoped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000/1500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">off-stoichiometric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of precursor solution preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass of the powder precursor weighted out in the glove box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of substance of precursor powder weighted out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume of solvent used to solve the powder precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass concentration of the prepared precursor-solvent solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount of substance concentration of the prepared precursor-solvent solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity of the precursor solution flow adjusted by peristaltic pumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># quantity description</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmol/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ml/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precursors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabrication date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume Solvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti-OiPr-2-tmhd-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:00+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr-tmhd-2-tetraglyme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La-tmhd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr/Ti ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation ratio of Sr and Ti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sr/La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation ratio of Sr and La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the chemical that is typically used in literature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the IUPAC nomencalture of the chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase of the chemical in ist bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabricating company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity of the Chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of the Invoice Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Opening the Chemical bottle in the Glove box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAS number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IUPAC Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buying date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of the first Precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titanium bis(isopropoxide) bis(2,2,6,6-tetramethylheptane-3,5-dionate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solid powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pegasus Chemicals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">144665-26-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of the second Precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bis(2,2,6,6-tetramethyl-3,5-heptanedionato)strontium 2,5,8,11,14-pentaoxapentadecane</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 150939-76-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification of the third Precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tris(2,2,6,6-tetramethyl-3,5-heptanedionato)lanthanum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14319-13-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample preparation including orientating, polishing, cutting done by this company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crystallographic orientation of the substrate in [hkl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off-cut angle to the substrates surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical doping level of electrically conductive substrates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doping species to obtain electrical conductivity in the substrates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate charge ID given by fabrication company. Detailed information can be obtained from the company by requesting this charge ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate dimensions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the sample annealed, cleaned and etched for smooth stepped surface?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was the substrate deposited already and is recycled by polishing?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wt.%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off-cut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doping Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doping species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recycled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First substrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrysTec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3202/8464/64 ML7272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 x 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second substrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3202/8854/63 ML6432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration of each step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Past time since process start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon process gas flow in to the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen process gas flow in to the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon gas in the flash evaporator used to push Ti-Precursor into the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon gas in the flash evaporator used to purge Ti-Precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature in the flash evaporation to vaporize the Ti-precursor solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure applied in the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature applied on the filament in the reaction chamber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature applied on the shaft in the reaction chamber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation velocity of the carrier with substrates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pumping velocity of the peristaltic pump of Ti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pumping velocity of the peristaltic pump of Sr/La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature in the flash evaporation to vaporize the Sr/La precursor solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon gas in the flash evaporator used to push Sr/La-Precursor into the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon gas in the flash evaporator used to purge Sr/La-Precursor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments in case irregularities occurred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sccm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon push Titan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon purge Titan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization temperature Titan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chamber pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaft temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrier rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peristaltic pump rotation Titan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peristaltic pump rotation Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization temperature Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon push Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon purge Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOVPE changes from Idle Mode to Deposition Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slow decrease of the chamber pressure to avoid damage in the turbo pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:02+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry Ag(liq)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heating step to dry liquid silver paste underneath the substrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:05+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrier rotation is started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:06+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stabilize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short stabilization steo to avoid damage in pumping system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:08+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activation of the peristaltic pumps. Precursor is supplied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:08:30+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooling down to room temperature after deposition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 10:09+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peristaltic pumps stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 11:19+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second step of cooling down to room temperature after deposition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 11:20+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop Gases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All gas flow is stopped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 11:35+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop Rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrier rotation is stopped and sample can be taken out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-15 11:38+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature that is controlled by the pyrometer on the substartes surface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization temperature of the Ti flash evaporator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization temperature of the Sr/La flash evaporator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen process gas temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backpressure in the Ti evaporation line controlling the vapor pressure of this line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backpressure in the Sr/La evaporation line controlling the vapor pressure of this line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening level of the hrottle valve at the turbo pump used to apply the chamber pressure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chamber pressure in the reaction chamber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carrier rottaion velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage control of the heating system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current control of the heating system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[°C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[mbar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[%]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[V]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[mA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># would you like this</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Stabwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># in the OVERVIEW?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyrotemperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization Ti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaporization Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2 temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backpressure Ti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backpressure Sr La</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throttle valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film thickness obtained from HRXRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vertical lattice parameter d_vert obtained from HRXRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[nm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Angstrom]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Start Time</t>
   </si>
   <si>
     <t xml:space="preserve">End Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity Method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Film</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2 Argon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22-01-21-MA-255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tarragona</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-08-25 10:33:25.013+02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:00+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epitaxy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Movpe sto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">giorgio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STO:La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 x STO undoped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2000/1500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">off-stoichiometric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of precursor solution preparation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass of the powder precursor weighted out in the glove box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount of substance of precursor powder weighted out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume of solvent used to solve the powder precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass concentration of the prepared precursor-solvent solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amount of substance concentration of the prepared precursor-solvent solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velocity of the precursor solution flow adjusted by peristaltic pumps</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># quantity description</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm/dd/yyyy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mmol/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precursors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabrication date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Solvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ti-OiPr-2-tmhd-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sr-tmhd-2-tetraglyme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La-tmhd-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sr/Ti ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cation ratio of Sr and Ti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sr/La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cation ratio of Sr and La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The name of the chemical that is typically used in literature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the IUPAC nomencalture of the chemical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase of the chemical in ist bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabricating company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purity of the Chemical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of the Invoice Mail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of Opening the Chemical bottle in the Glove box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IUPAC Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buying date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opening date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specification of the first Precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium bis(isopropoxide) bis(2,2,6,6-tetramethylheptane-3,5-dionate)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solid powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pegasus Chemicals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">144665-26-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specification of the second Precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bis(2,2,6,6-tetramethyl-3,5-heptanedionato)strontium 2,5,8,11,14-pentaoxapentadecane</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 150939-76-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specification of the third Precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tris(2,2,6,6-tetramethyl-3,5-heptanedionato)lanthanum</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14319-13-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample preparation including orientating, polishing, cutting done by this company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crystallographic orientation of the substrate in [hkl]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off-cut angle to the substrates surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical doping level of electrically conductive substrates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doping species to obtain electrical conductivity in the substrates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate charge ID given by fabrication company. Detailed information can be obtained from the company by requesting this charge ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate dimensions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the sample annealed, cleaned and etched for smooth stepped surface?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was the substrate deposited already and is recycled by polishing?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">°</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wt.%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm²</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># str</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orientation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off-cut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doping Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doping species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recycled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First substrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrysTec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3202/8464/64 ML7272</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 x 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second substrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3202/8854/63 ML6432</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration of each step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Past time since process start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon process gas flow in to the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen process gas flow in to the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon gas in the flash evaporator used to push Ti-Precursor into the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon gas in the flash evaporator used to purge Ti-Precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature in the flash evaporation to vaporize the Ti-precursor solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure applied in the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature applied on the filament in the reaction chamber </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature applied on the shaft in the reaction chamber </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation velocity of the carrier with substrates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pumping velocity of the peristaltic pump of Ti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pumping velocity of the peristaltic pump of Sr/La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature in the flash evaporation to vaporize the Sr/La precursor solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon gas in the flash evaporator used to push Sr/La-Precursor into the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon gas in the flash evaporator used to purge Sr/La-Precursor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments in case irregularities occurred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sccm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">°C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rpm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon push Titan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon purge Titan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization temperature Titan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chamber pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaft temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrier rotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peristaltic pump rotation Titan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peristaltic pump rotation Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization temperature Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon push Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argon purge Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annotations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initialize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOVPE changes from Idle Mode to Deposition Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slow decrease of the chamber pressure to avoid damage in the turbo pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:02+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Ag(liq)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heating step to dry liquid silver paste underneath the substrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:05+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strong deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrier rotation is started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:06+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stabilize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short stabilization steo to avoid damage in pumping system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:08+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activation of the peristaltic pumps. Precursor is supplied.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:08:30+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooling down to room temperature after deposition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 10:09+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop pump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peristaltic pumps stop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 11:19+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Second step of cooling down to room temperature after deposition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 11:20+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop Gases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All gas flow is stopped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 11:35+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop Rotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrier rotation is stopped and sample can be taken out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-15 11:38+01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperature that is controlled by the pyrometer on the substartes surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization temperature of the Ti flash evaporator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization temperature of the Sr/La flash evaporator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen process gas temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backpressure in the Ti evaporation line controlling the vapor pressure of this line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backpressure in the Sr/La evaporation line controlling the vapor pressure of this line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opening level of the hrottle valve at the turbo pump used to apply the chamber pressure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">chamber pressure in the reaction chamber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carrier rottaion velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage control of the heating system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current control of the heating system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[°C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[mbar]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[%]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[V]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[mA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Average</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># would you like this</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Stabwa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># in the OVERVIEW?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyrotemperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization Ti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaporization Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2 temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backpressure Ti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backpressure Sr La</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Throttle valve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Film thickness obtained from HRXRD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertical lattice parameter d_vert obtained from HRXRD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[nm]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Angstrom]</t>
   </si>
   <si>
     <t xml:space="preserve">Thickness</t>
@@ -822,15 +822,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="#,##0"/>
+    <numFmt numFmtId="169" formatCode="#,##0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1013,7 +1011,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1250,27 +1248,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1353,8 +1331,8 @@
   </sheetPr>
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1362,19 +1340,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="33.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="39.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="39.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,10 +1369,9 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -1406,30 +1383,29 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -1439,26 +1415,23 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
@@ -1470,7 +1443,9 @@
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="G4" s="9" t="s">
         <v>16</v>
       </c>
@@ -1478,22 +1453,19 @@
         <v>16</v>
       </c>
       <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -1509,10 +1481,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
     </row>
     <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
@@ -1548,53 +1519,48 @@
       <c r="K6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="11" t="s">
-        <v>31</v>
-      </c>
+      <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="R6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -1609,9 +1575,8 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -1626,9 +1591,8 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -1642,10 +1606,9 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -1659,10 +1622,9 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -1676,10 +1638,9 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1735,55 +1696,55 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>14</v>
@@ -1791,7 +1752,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -1834,42 +1795,42 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="E6" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="G6" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="H6" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="I6" s="21" t="s">
         <v>65</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>35</v>
       </c>
       <c r="D7" s="24" t="n">
         <f aca="false">0.3061*1000</f>
@@ -1896,13 +1857,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C8" s="23" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D8" s="24" t="n">
         <f aca="false">0.1929*1000</f>
@@ -1929,13 +1890,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="C9" s="23" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D9" s="24" t="n">
         <v>3.5</v>
@@ -1961,10 +1922,10 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="24" t="n">
@@ -1982,10 +1943,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="24" t="n">
@@ -2058,41 +2019,41 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="6"/>
@@ -2101,10 +2062,10 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="3" t="s">
@@ -2114,7 +2075,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>16</v>
@@ -2166,34 +2127,34 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="H6" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="J6" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>94</v>
       </c>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
@@ -2212,102 +2173,102 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -2383,38 +2344,38 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="E2" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="F2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="G2" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="H2" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="I2" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="J2" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="K2" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="36" t="s">
-        <v>115</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -3431,21 +3392,21 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>116</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>117</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J3" s="39"/>
       <c r="K3" s="39"/>
@@ -3456,7 +3417,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>16</v>
@@ -3512,111 +3473,111 @@
     </row>
     <row r="6" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="42" t="s">
+      <c r="E6" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="F6" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="G6" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="H6" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="I6" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="J6" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="K6" s="42" t="s">
         <v>127</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>128</v>
       </c>
       <c r="L6" s="35"/>
       <c r="M6" s="35"/>
     </row>
     <row r="7" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>130</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>131</v>
       </c>
       <c r="D7" s="43" t="n">
         <v>-100</v>
       </c>
       <c r="E7" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="G7" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="H7" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="I7" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="J7" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="K7" s="43" t="s">
         <v>137</v>
-      </c>
-      <c r="K7" s="43" t="s">
-        <v>138</v>
       </c>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
     </row>
     <row r="8" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>140</v>
-      </c>
       <c r="C8" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="43" t="n">
         <v>-100</v>
       </c>
       <c r="E8" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>142</v>
-      </c>
       <c r="I8" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="K8" s="43" t="s">
         <v>137</v>
-      </c>
-      <c r="K8" s="43" t="s">
-        <v>138</v>
       </c>
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
@@ -3897,58 +3858,58 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="U2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3960,52 +3921,52 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="K3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="N3" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>162</v>
-      </c>
       <c r="R3" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T3" s="6"/>
       <c r="U3" s="3" t="s">
@@ -4014,13 +3975,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>17</v>
@@ -4029,31 +3990,31 @@
         <v>15</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>17</v>
@@ -4062,13 +4023,13 @@
         <v>17</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>16</v>
@@ -4105,64 +4066,64 @@
     </row>
     <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="C6" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="52" t="s">
+      <c r="E6" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="G6" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="52" t="s">
+      <c r="H6" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="I6" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="J6" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="I6" s="52" t="s">
+      <c r="K6" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="L6" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="M6" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="L6" s="52" t="s">
+      <c r="N6" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="M6" s="52" t="s">
+      <c r="O6" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="P6" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="O6" s="52" t="s">
+      <c r="Q6" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="R6" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="Q6" s="52" t="s">
+      <c r="S6" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="R6" s="52" t="s">
+      <c r="T6" s="52" t="s">
         <v>183</v>
-      </c>
-      <c r="S6" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="T6" s="52" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,16 +4131,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>100</v>
@@ -4224,7 +4185,7 @@
         <v>450</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4232,16 +4193,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>100</v>
@@ -4286,7 +4247,7 @@
         <v>450</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4294,16 +4255,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>1500</v>
@@ -4348,7 +4309,7 @@
         <v>450</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4356,16 +4317,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1500</v>
@@ -4410,7 +4371,7 @@
         <v>450</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4418,16 +4379,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>1500</v>
@@ -4472,7 +4433,7 @@
         <v>450</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,16 +4441,16 @@
         <v>9</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>1500</v>
@@ -4534,7 +4495,7 @@
         <v>450</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4542,16 +4503,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D13" s="56" t="n">
         <v>70</v>
       </c>
       <c r="E13" s="54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F13" s="56" t="n">
         <v>1500</v>
@@ -4596,7 +4557,7 @@
         <v>450</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4604,16 +4565,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F14" s="2" t="n">
         <v>1000</v>
@@ -4658,7 +4619,7 @@
         <v>450</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4666,16 +4627,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C15" s="55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>15</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>1000</v>
@@ -4720,7 +4681,7 @@
         <v>450</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4728,16 +4689,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>3</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>1000</v>
@@ -4782,7 +4743,7 @@
         <v>450</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4790,16 +4751,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>100</v>
@@ -4844,7 +4805,7 @@
         <v>450</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4874,39 +4835,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BJ13"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="32.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="8.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="8.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -4918,93 +4878,96 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>50</v>
+      <c r="O2" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="K3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5012,11 +4975,9 @@
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>17</v>
@@ -5048,7 +5009,10 @@
       <c r="M4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5056,10 +5020,8 @@
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5070,386 +5032,340 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="B6" s="0"/>
-      <c r="C6" s="57" t="n">
-        <f aca="false">AVERAGE(C10:C13)</f>
+        <v>233</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="57" t="n">
+        <f aca="false">AVERAGE(D10:D12)</f>
         <v>736.666666666667</v>
       </c>
-      <c r="D6" s="57" t="n">
-        <f aca="false">AVERAGE(D10:D13)</f>
+      <c r="E6" s="57" t="n">
+        <f aca="false">AVERAGE(E10:E12)</f>
         <v>215</v>
       </c>
-      <c r="E6" s="57" t="n">
-        <f aca="false">AVERAGE(E10:E13)</f>
+      <c r="F6" s="57" t="n">
+        <f aca="false">AVERAGE(F10:F12)</f>
         <v>213</v>
       </c>
-      <c r="F6" s="57" t="n">
-        <f aca="false">AVERAGE(F10:F13)</f>
+      <c r="G6" s="57" t="n">
+        <f aca="false">AVERAGE(G10:G12)</f>
         <v>70.6333333333333</v>
       </c>
-      <c r="G6" s="57" t="n">
-        <f aca="false">AVERAGE(G10:G13)</f>
+      <c r="H6" s="57" t="n">
+        <f aca="false">AVERAGE(H10:H12)</f>
         <v>29.0666666666667</v>
       </c>
-      <c r="H6" s="57" t="n">
-        <f aca="false">AVERAGE(H10:H13)</f>
+      <c r="I6" s="57" t="n">
+        <f aca="false">AVERAGE(I10:I12)</f>
         <v>33.2333333333333</v>
       </c>
-      <c r="I6" s="57" t="n">
-        <f aca="false">AVERAGE(I10:I13)</f>
+      <c r="J6" s="57" t="n">
+        <f aca="false">AVERAGE(J10:J12)</f>
         <v>44.3666666666667</v>
       </c>
-      <c r="J6" s="57" t="n">
-        <f aca="false">AVERAGE(J10:J13)</f>
+      <c r="K6" s="57" t="n">
+        <f aca="false">AVERAGE(K10:K12)</f>
         <v>15.2</v>
       </c>
-      <c r="K6" s="57" t="n">
-        <f aca="false">AVERAGE(K10:K13)</f>
+      <c r="L6" s="57" t="n">
+        <f aca="false">AVERAGE(L10:L12)</f>
         <v>623</v>
       </c>
-      <c r="L6" s="57" t="n">
-        <f aca="false">AVERAGE(L10:L13)</f>
+      <c r="M6" s="57" t="n">
+        <f aca="false">AVERAGE(M10:M12)</f>
         <v>16.6666666666667</v>
       </c>
-      <c r="M6" s="57" t="n">
-        <f aca="false">AVERAGE(M10:M13)</f>
+      <c r="N6" s="57" t="n">
+        <f aca="false">AVERAGE(N10:N12)</f>
         <v>43.6666666666667</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>236</v>
+      <c r="O6" s="3" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="57" t="n">
-        <f aca="false">STDEVA(C10:C13)</f>
+        <v>235</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="57" t="n">
+        <f aca="false">STDEVA(D10:D12)</f>
         <v>1.15470053837925</v>
       </c>
-      <c r="D7" s="57" t="n">
-        <f aca="false">STDEVA(D10:D13)</f>
+      <c r="E7" s="57" t="n">
+        <f aca="false">STDEVA(E10:E12)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="57" t="n">
-        <f aca="false">STDEVA(E10:E13)</f>
+      <c r="F7" s="57" t="n">
+        <f aca="false">STDEVA(F10:F12)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="57" t="n">
-        <f aca="false">STDEVA(F10:F13)</f>
+      <c r="G7" s="57" t="n">
+        <f aca="false">STDEVA(G10:G12)</f>
         <v>0.305505046330394</v>
       </c>
-      <c r="G7" s="57" t="n">
-        <f aca="false">STDEVA(G10:G13)</f>
+      <c r="H7" s="57" t="n">
+        <f aca="false">STDEVA(H10:H12)</f>
         <v>0.404145188432738</v>
       </c>
-      <c r="H7" s="57" t="n">
-        <f aca="false">STDEVA(H10:H13)</f>
+      <c r="I7" s="57" t="n">
+        <f aca="false">STDEVA(I10:I12)</f>
         <v>1.98578280114753</v>
       </c>
-      <c r="I7" s="57" t="n">
-        <f aca="false">STDEVA(I10:I13)</f>
+      <c r="J7" s="57" t="n">
+        <f aca="false">STDEVA(J10:J12)</f>
         <v>1.53079500042734</v>
       </c>
-      <c r="J7" s="57" t="n">
-        <f aca="false">STDEVA(J10:J13)</f>
+      <c r="K7" s="57" t="n">
+        <f aca="false">STDEVA(K10:K12)</f>
         <v>1.05830052442584</v>
       </c>
-      <c r="K7" s="57" t="n">
-        <f aca="false">STDEVA(K10:K13)</f>
+      <c r="L7" s="57" t="n">
+        <f aca="false">STDEVA(L10:L12)</f>
         <v>10.5356537528527</v>
       </c>
-      <c r="L7" s="57" t="n">
-        <f aca="false">STDEVA(L10:L13)</f>
+      <c r="M7" s="57" t="n">
+        <f aca="false">STDEVA(M10:M12)</f>
         <v>0.577350269189626</v>
       </c>
-      <c r="M7" s="57" t="n">
-        <f aca="false">STDEVA(M10:M13)</f>
+      <c r="N7" s="57" t="n">
+        <f aca="false">STDEVA(N10:N12)</f>
         <v>0.577350269189626</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>238</v>
+      <c r="O7" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="G8" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="H8" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="I8" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="J8" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="K8" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="M8" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="N8" s="20" t="s">
         <v>245</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C9" s="58" t="n">
+      <c r="D9" s="58" t="n">
         <v>725</v>
       </c>
-      <c r="D9" s="58" t="n">
+      <c r="E9" s="58" t="n">
         <v>215</v>
       </c>
-      <c r="E9" s="58" t="n">
+      <c r="F9" s="58" t="n">
         <v>213</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="G9" s="2" t="n">
         <v>70</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="H9" s="2" t="n">
         <v>30.6</v>
       </c>
-      <c r="H9" s="58" t="n">
+      <c r="I9" s="58" t="n">
         <v>35.2</v>
       </c>
-      <c r="I9" s="58" t="n">
+      <c r="J9" s="58" t="n">
         <v>40.6</v>
       </c>
-      <c r="J9" s="58" t="n">
+      <c r="K9" s="58" t="n">
         <v>15.6</v>
       </c>
-      <c r="K9" s="58" t="n">
+      <c r="L9" s="58" t="n">
         <v>627</v>
       </c>
-      <c r="L9" s="58" t="n">
+      <c r="M9" s="58" t="n">
         <v>16</v>
       </c>
-      <c r="M9" s="58" t="n">
+      <c r="N9" s="58" t="n">
         <v>43</v>
       </c>
-      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B10" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="C10" s="58" t="n">
+      <c r="D10" s="58" t="n">
         <v>736</v>
       </c>
-      <c r="D10" s="58" t="n">
+      <c r="E10" s="58" t="n">
         <v>215</v>
       </c>
-      <c r="E10" s="58" t="n">
+      <c r="F10" s="58" t="n">
         <v>213</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="G10" s="2" t="n">
         <v>70.3</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="H10" s="2" t="n">
         <v>29.3</v>
       </c>
-      <c r="H10" s="58" t="n">
+      <c r="I10" s="58" t="n">
         <v>34.8</v>
       </c>
-      <c r="I10" s="58" t="n">
+      <c r="J10" s="58" t="n">
         <v>43.8</v>
       </c>
-      <c r="J10" s="58" t="n">
+      <c r="K10" s="58" t="n">
         <v>16</v>
       </c>
-      <c r="K10" s="58" t="n">
+      <c r="L10" s="58" t="n">
         <v>624</v>
       </c>
-      <c r="L10" s="58" t="n">
+      <c r="M10" s="58" t="n">
         <v>17</v>
       </c>
-      <c r="M10" s="58" t="n">
+      <c r="N10" s="58" t="n">
         <v>44</v>
       </c>
-      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="C11" s="58" t="n">
+      <c r="D11" s="58" t="n">
         <v>736</v>
       </c>
-      <c r="D11" s="58" t="n">
+      <c r="E11" s="58" t="n">
         <v>215</v>
       </c>
-      <c r="E11" s="58" t="n">
+      <c r="F11" s="58" t="n">
         <v>213</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="G11" s="2" t="n">
         <v>70.7</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="H11" s="2" t="n">
         <v>29.3</v>
       </c>
-      <c r="H11" s="58" t="n">
+      <c r="I11" s="58" t="n">
         <v>33.9</v>
       </c>
-      <c r="I11" s="58" t="n">
+      <c r="J11" s="58" t="n">
         <v>43.2</v>
       </c>
-      <c r="J11" s="58" t="n">
+      <c r="K11" s="58" t="n">
         <v>15.6</v>
       </c>
-      <c r="K11" s="58" t="n">
+      <c r="L11" s="58" t="n">
         <v>633</v>
       </c>
-      <c r="L11" s="58" t="n">
+      <c r="M11" s="58" t="n">
         <v>16</v>
       </c>
-      <c r="M11" s="58" t="n">
+      <c r="N11" s="58" t="n">
         <v>43</v>
       </c>
-      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="C12" s="58" t="n">
+      <c r="D12" s="58" t="n">
         <v>738</v>
       </c>
-      <c r="D12" s="58" t="n">
+      <c r="E12" s="58" t="n">
         <v>215</v>
       </c>
-      <c r="E12" s="58" t="n">
+      <c r="F12" s="58" t="n">
         <v>213</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="G12" s="2" t="n">
         <v>70.9</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="H12" s="2" t="n">
         <v>28.6</v>
       </c>
-      <c r="H12" s="58" t="n">
+      <c r="I12" s="58" t="n">
         <v>31</v>
       </c>
-      <c r="I12" s="58" t="n">
+      <c r="J12" s="58" t="n">
         <v>46.1</v>
       </c>
-      <c r="J12" s="58" t="n">
+      <c r="K12" s="58" t="n">
         <v>14</v>
       </c>
-      <c r="K12" s="58" t="n">
+      <c r="L12" s="58" t="n">
         <v>612</v>
       </c>
-      <c r="L12" s="58" t="n">
+      <c r="M12" s="58" t="n">
         <v>17</v>
       </c>
-      <c r="M12" s="58" t="n">
+      <c r="N12" s="58" t="n">
         <v>44</v>
       </c>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="62"/>
-      <c r="U13" s="62"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="63"/>
-      <c r="X13" s="63"/>
-      <c r="Y13" s="63"/>
-      <c r="Z13" s="63"/>
-      <c r="AA13" s="63"/>
-      <c r="AB13" s="63"/>
-      <c r="AC13" s="63"/>
-      <c r="AD13" s="63"/>
-      <c r="AE13" s="63"/>
-      <c r="AF13" s="63"/>
-      <c r="AG13" s="63"/>
-      <c r="AH13" s="63"/>
-      <c r="AI13" s="63"/>
-      <c r="AJ13" s="63"/>
-      <c r="AK13" s="63"/>
-      <c r="AL13" s="63"/>
-      <c r="AM13" s="63"/>
-      <c r="AN13" s="63"/>
-      <c r="AO13" s="63"/>
-      <c r="AP13" s="63"/>
-      <c r="AQ13" s="63"/>
-      <c r="AR13" s="63"/>
-      <c r="AS13" s="63"/>
-      <c r="AT13" s="63"/>
-      <c r="AU13" s="63"/>
-      <c r="AV13" s="63"/>
-      <c r="AW13" s="63"/>
-      <c r="AX13" s="63"/>
-      <c r="AY13" s="63"/>
-      <c r="AZ13" s="63"/>
-      <c r="BA13" s="63"/>
-      <c r="BB13" s="63"/>
-      <c r="BC13" s="63"/>
-      <c r="BD13" s="63"/>
-      <c r="BE13" s="63"/>
-      <c r="BF13" s="63"/>
-      <c r="BG13" s="63"/>
-      <c r="BH13" s="63"/>
-      <c r="BI13" s="63"/>
-      <c r="BJ13" s="63"/>
+      <c r="O12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5510,10 +5426,10 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>9</v>
@@ -5533,10 +5449,10 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>14</v>
@@ -5590,16 +5506,16 @@
         <v>21</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>256</v>
@@ -5611,16 +5527,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>258</v>
@@ -5631,7 +5547,7 @@
       <c r="G7" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="H7" s="64" t="n">
+      <c r="H7" s="59" t="n">
         <v>3961</v>
       </c>
       <c r="I7" s="3"/>
@@ -5765,7 +5681,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>14</v>
@@ -5815,16 +5731,16 @@
         <v>21</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
       <c r="D6" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>261</v>
@@ -5833,16 +5749,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>258</v>

</xml_diff>

<commit_message>
added Instrument link into Activity, updated the MOVPE_STO schema
</commit_message>
<xml_diff>
--- a/movpe_STO/datafile.xlsx
+++ b/movpe_STO/datafile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="266">
   <si>
     <t xml:space="preserve">########## start Header ##########</t>
   </si>
@@ -791,10 +791,13 @@
     <t xml:space="preserve">[Angstrom]</t>
   </si>
   <si>
-    <t xml:space="preserve">Start Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End Time</t>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method</t>
   </si>
   <si>
     <t xml:space="preserve">Thickness</t>
@@ -803,6 +806,9 @@
     <t xml:space="preserve">d Vertical</t>
   </si>
   <si>
+    <t xml:space="preserve">Dresden</t>
+  </si>
+  <si>
     <t xml:space="preserve">measurement</t>
   </si>
   <si>
@@ -813,6 +819,9 @@
   </si>
   <si>
     <t xml:space="preserve">Roughness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berlin</t>
   </si>
   <si>
     <t xml:space="preserve">0.6</t>
@@ -830,7 +839,7 @@
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -893,12 +902,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1228,7 +1231,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1331,7 +1334,7 @@
   </sheetPr>
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1352,7 +1355,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="39.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1525,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="R6" s="0"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -4843,13 +4846,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="8.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.29"/>
@@ -5040,7 +5043,7 @@
         <v>233</v>
       </c>
       <c r="B6" s="56"/>
-      <c r="C6" s="0"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="57" t="n">
         <f aca="false">AVERAGE(D10:D12)</f>
         <v>736.666666666667</v>
@@ -5094,7 +5097,7 @@
         <v>235</v>
       </c>
       <c r="B7" s="56"/>
-      <c r="C7" s="0"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="57" t="n">
         <f aca="false">STDEVA(D10:D12)</f>
         <v>1.15470053837925</v>
@@ -5383,10 +5386,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5394,11 +5397,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="46.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="46.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5411,8 +5414,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -5424,14 +5426,13 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5443,18 +5444,15 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="G3" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="H3" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5467,21 +5465,18 @@
         <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5495,62 +5490,55 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>254</v>
+        <v>22</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>255</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>23</v>
+        <v>256</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>24</v>
+        <v>257</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="I6" s="12"/>
+        <v>258</v>
+      </c>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>259</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>68</v>
+      <c r="D7" s="14" t="s">
+        <v>260</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="G7" s="2" t="n">
+        <v>261</v>
+      </c>
+      <c r="F7" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="H7" s="59" t="n">
+      <c r="G7" s="59" t="n">
         <v>3961</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -5561,7 +5549,6 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -5572,7 +5559,6 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -5582,7 +5568,6 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -5592,7 +5577,6 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -5602,7 +5586,6 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5620,10 +5603,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5631,10 +5614,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5646,8 +5629,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -5659,11 +5641,10 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5675,15 +5656,12 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5696,18 +5674,15 @@
         <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5720,56 +5695,49 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>254</v>
+        <v>22</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>255</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>23</v>
+        <v>256</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="H6" s="12"/>
+        <v>263</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>264</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>68</v>
+      <c r="D7" s="14" t="s">
+        <v>260</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H7" s="3"/>
+        <v>261</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -5779,7 +5747,6 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -5789,28 +5756,24 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>